<commit_message>
add FB_Power and some diffs in FB_Thermal, FB_Main and Data Structure
</commit_message>
<xml_diff>
--- a/Resources/数据帧格式.xlsx
+++ b/Resources/数据帧格式.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSS\FlyingBlocks\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\学习\桌面卫星\Desk_Sate_Code\FlyingBlocks\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F2A183-EFA4-435F-BF31-C65CE5C4C230}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23130" windowHeight="10395"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,10 +98,6 @@
     <t>0x01</t>
   </si>
   <si>
-    <t>0x00 关闭电源控制
-0x01 打开电源控制</t>
-  </si>
-  <si>
     <t>飞轮控制开关</t>
   </si>
   <si>
@@ -248,12 +245,31 @@
 byte[28:39]: 包含 3 个元素的 float 型数组，三个元素分别表示三轴加速度</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>byte[5]: 0x00 电源开关0关闭
+             0x01 电源开关0打开
+byte[6]: 0x00 电源开关1关闭
+             0x01 电源开关1打开
+byte[7]: 0x00 电源开关2关闭
+             0x01 电源开关2打开
+byte[8]: 0x00 电源开关3关闭
+             0x01 电源开关3打开
+byte[9]: 0x00 电源开关4关闭
+             0x01 电源开关4打开
+byte[10]: 0x00 电源开关5关闭
+               0x01 电源开关5打开
+byte[11]: 0x00 电源开关6关闭
+               0x01 电源开关6打开
+byte[12]: 0x00 电源开关7关闭
+               0x01 电源开关7打开</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +288,13 @@
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -346,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -401,6 +424,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -420,7 +446,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -495,6 +521,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -530,6 +573,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -705,28 +765,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.62890625" defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="6"/>
-    <col min="2" max="2" width="16.375" style="6" customWidth="1"/>
-    <col min="3" max="4" width="8.625" style="6"/>
+    <col min="1" max="1" width="8.62890625" style="6"/>
+    <col min="2" max="2" width="16.3671875" style="6" customWidth="1"/>
+    <col min="3" max="4" width="8.62890625" style="6"/>
     <col min="5" max="5" width="10" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.89453125" style="6" customWidth="1"/>
     <col min="7" max="7" width="36" style="7" customWidth="1"/>
-    <col min="8" max="8" width="15.25" style="6" customWidth="1"/>
-    <col min="9" max="9" width="11.625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.625" style="6"/>
+    <col min="8" max="8" width="15.26171875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="11.62890625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="11.47265625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.62890625" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
@@ -739,7 +799,7 @@
       <c r="I2" s="12"/>
       <c r="J2" s="13"/>
     </row>
-    <row r="3" spans="2:10" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:10" ht="28.2" x14ac:dyDescent="0.4">
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
@@ -764,7 +824,7 @@
       </c>
       <c r="J3" s="14"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
         <v>8</v>
@@ -791,7 +851,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B5" s="9" t="s">
         <v>16</v>
       </c>
@@ -820,7 +880,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:10" ht="225.6" x14ac:dyDescent="0.4">
       <c r="B6" s="9" t="s">
         <v>23</v>
       </c>
@@ -836,8 +896,8 @@
       <c r="F6" s="8">
         <v>1</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>25</v>
+      <c r="G6" s="19" t="s">
+        <v>64</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>20</v>
@@ -849,9 +909,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:10" ht="28.2" x14ac:dyDescent="0.4">
       <c r="B7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>17</v>
@@ -860,13 +920,13 @@
         <v>18</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="8">
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>20</v>
@@ -878,9 +938,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:10" ht="28.2" x14ac:dyDescent="0.4">
       <c r="B8" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>17</v>
@@ -889,13 +949,13 @@
         <v>18</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="8">
         <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>20</v>
@@ -907,9 +967,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:10" ht="28.2" x14ac:dyDescent="0.4">
       <c r="B9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>17</v>
@@ -918,13 +978,13 @@
         <v>18</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="8">
         <v>1</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>20</v>
@@ -936,9 +996,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:10" ht="28.2" x14ac:dyDescent="0.4">
       <c r="B10" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>17</v>
@@ -947,13 +1007,13 @@
         <v>18</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="8">
         <v>1</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>20</v>
@@ -965,9 +1025,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="57" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:10" ht="112.8" x14ac:dyDescent="0.4">
       <c r="B11" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>17</v>
@@ -976,13 +1036,13 @@
         <v>18</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="8">
         <v>16</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>20</v>
@@ -994,9 +1054,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="57" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:10" ht="56.4" x14ac:dyDescent="0.4">
       <c r="B12" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>17</v>
@@ -1005,13 +1065,13 @@
         <v>18</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="8">
         <v>3</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H12" s="8" t="s">
         <v>20</v>
@@ -1023,9 +1083,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:10" ht="71.099999999999994" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B14" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -1036,7 +1097,7 @@
       <c r="I14" s="12"/>
       <c r="J14" s="13"/>
     </row>
-    <row r="15" spans="2:10" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:10" ht="28.2" x14ac:dyDescent="0.4">
       <c r="B15" s="8" t="s">
         <v>1</v>
       </c>
@@ -1048,7 +1109,7 @@
         <v>3</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>5</v>
@@ -1061,7 +1122,7 @@
       </c>
       <c r="J15" s="14"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
         <v>8</v>
@@ -1088,9 +1149,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="42.75" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:10" ht="42.3" x14ac:dyDescent="0.4">
       <c r="B17" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>17</v>
@@ -1105,7 +1166,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>20</v>
@@ -1117,9 +1178,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:10" ht="84.6" x14ac:dyDescent="0.4">
       <c r="B18" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>17</v>
@@ -1128,13 +1189,13 @@
         <v>18</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F18" s="8">
         <v>17</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>20</v>
@@ -1146,9 +1207,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="85.5" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:10" ht="84.6" x14ac:dyDescent="0.4">
       <c r="B19" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>17</v>
@@ -1157,13 +1218,13 @@
         <v>18</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="8">
         <v>36</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>20</v>
@@ -1175,9 +1236,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="42.75" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:10" ht="42.3" x14ac:dyDescent="0.4">
       <c r="B20" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>17</v>
@@ -1186,13 +1247,13 @@
         <v>18</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20" s="8">
         <v>3</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>20</v>
@@ -1204,9 +1265,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="114" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:10" ht="112.8" x14ac:dyDescent="0.4">
       <c r="B21" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>17</v>
@@ -1215,13 +1276,13 @@
         <v>18</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F21" s="8">
         <v>7</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>20</v>
@@ -1233,17 +1294,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B22" s="10"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:10" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="2:10" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:10" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G25" s="2"/>
     </row>
   </sheetData>
@@ -1257,149 +1318,149 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.62890625" defaultRowHeight="14.1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="1"/>
-    <col min="2" max="2" width="16.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.62890625" style="1"/>
+    <col min="2" max="2" width="16.3671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1015625" style="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.75" style="2" customWidth="1"/>
-    <col min="8" max="8" width="11.125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.625" style="1"/>
+    <col min="6" max="6" width="12.89453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.1015625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.62890625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.47265625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.62890625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B2" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="17"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:7" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:7" ht="28.2" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="2:7" ht="56.4" x14ac:dyDescent="0.4">
+      <c r="B4" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="2:7" ht="57" x14ac:dyDescent="0.15">
-      <c r="B4" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B6" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="28.2" x14ac:dyDescent="0.4">
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="B8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:7" ht="28.2" x14ac:dyDescent="0.4">
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.15">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B11" s="2"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.4">
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.4">
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.4">
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B21" s="2"/>
     </row>
-    <row r="24" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="24" spans="2:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:D2"/>

</xml_diff>